<commit_message>
Bloqué au delete de la queue
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Documents\UiPath\Queue Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A15DEF-1DF8-4F13-9A13-05A83C600BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C83EF73-7196-487E-AD30-25435603F816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,38 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>QueueName</t>
+  </si>
+  <si>
+    <t>YearlyReport</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -55,8 +83,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,14 +366,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" customWidth="1"/>
+    <col min="3" max="3" width="45.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>